<commit_message>
part list propably finalized
</commit_message>
<xml_diff>
--- a/parts.xlsx
+++ b/parts.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>NUMBER OF BOARDS</t>
   </si>
@@ -54,30 +54,9 @@
     <t>count per one board</t>
   </si>
   <si>
-    <t>socket</t>
-  </si>
-  <si>
     <t>current</t>
   </si>
   <si>
-    <t>sockets</t>
-  </si>
-  <si>
-    <t>SOCKETS TO BUY</t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/cz/en/details/zl262-8sg/pin-headers/connfly/ds1023-1-8s21/</t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/cz/en/details/zl262-2sg/pin-headers/connfly/ds1023-1-2s21/</t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/cz/en/details/zl307-1x1/pin-headers/connfly/ds1002-03-1-1131/</t>
-  </si>
-  <si>
-    <t>wires</t>
-  </si>
-  <si>
     <t>control electronics</t>
   </si>
   <si>
@@ -87,18 +66,9 @@
     <t>https://www.tme.eu/cz/en/details/zl201-16g/pin-headers/connfly/ds1021-1-16sf11/</t>
   </si>
   <si>
-    <t>potencio</t>
-  </si>
-  <si>
     <t>piezzo</t>
   </si>
   <si>
-    <t>https://www.tme.eu/cz/details/lpb1475b-to-12/piezosireny-s-generatorem/cre-sound-electronics/lpb1475b-to-12-4-0-7-6-r-lab/</t>
-  </si>
-  <si>
-    <t>piezzo R</t>
-  </si>
-  <si>
     <t>button</t>
   </si>
   <si>
@@ -111,10 +81,43 @@
     <t>https://www.tme.eu/cz/en/details/fyl-5013hd1c/tht-leds-5mm/foryard/</t>
   </si>
   <si>
-    <t>LED R</t>
-  </si>
-  <si>
     <t>mega-bomb cable</t>
+  </si>
+  <si>
+    <t>4 dip switch</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/cz/en/details/sda04h0sb/dip-switches/c-k/</t>
+  </si>
+  <si>
+    <t>wires female</t>
+  </si>
+  <si>
+    <t>headers</t>
+  </si>
+  <si>
+    <t>HEADERS TO BUY</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/cz/en/details/zl201-08g/pin-headers/connfly/ds1021-1-8sf11-b/</t>
+  </si>
+  <si>
+    <t>TOTAL HEADERS</t>
+  </si>
+  <si>
+    <t>piezzo 1kR</t>
+  </si>
+  <si>
+    <t>LED 330 R</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/cz/details/bpt-14x/piezosireny-s-generatorem/bestar/bpt14x/</t>
+  </si>
+  <si>
+    <t>BUY</t>
+  </si>
+  <si>
+    <t>HEADER 8</t>
   </si>
 </sst>
 </file>
@@ -138,7 +141,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,6 +157,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -174,7 +183,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -192,6 +201,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -489,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -501,21 +516,23 @@
     <col min="2" max="2" width="14.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="77.140625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="14.42578125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -524,7 +541,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:10">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -537,10 +554,10 @@
       </c>
       <c r="E3" s="3">
         <f>$D$1*C3</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -552,11 +569,11 @@
         <v>4</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" ref="E4:E17" si="0">$D$1*C4</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <f t="shared" ref="E4:E6" si="0">$D$1*C4</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>6</v>
@@ -569,10 +586,10 @@
       </c>
       <c r="E5" s="3">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>8</v>
@@ -585,17 +602,23 @@
       </c>
       <c r="E6" s="3">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="G7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>10</v>
@@ -605,10 +628,21 @@
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="G8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="7">
+        <f xml:space="preserve"> ROUNDUP($C$17/8, 0)*$D$1</f>
+        <v>11</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
@@ -621,10 +655,21 @@
         <v>16</v>
       </c>
       <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="G9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="7">
+        <f>E3+E4+E34+E31</f>
+        <v>11</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2">
         <v>2</v>
@@ -637,10 +682,21 @@
         <v>12</v>
       </c>
       <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="G10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="7">
+        <f>E5</f>
+        <v>2</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2">
         <v>3</v>
@@ -653,10 +709,21 @@
         <v>6</v>
       </c>
       <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="G11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="7">
+        <f>E6</f>
+        <v>1</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2">
         <v>4</v>
@@ -669,10 +736,21 @@
         <v>4</v>
       </c>
       <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="G12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="7">
+        <f>E29</f>
+        <v>1</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B13" s="2">
         <v>8</v>
@@ -685,11 +763,22 @@
         <v>16</v>
       </c>
       <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="G13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="7">
+        <f>E30</f>
+        <v>1</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2">
@@ -697,233 +786,285 @@
         <v>54</v>
       </c>
       <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="G14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="7">
+        <f>E32</f>
+        <v>1</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2">
         <v>54</v>
       </c>
       <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="G15" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="7">
+        <f>E33</f>
+        <v>1</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="3"/>
-      <c r="B17" s="3">
-        <v>8</v>
+      <c r="B17" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="C17" s="3">
-        <v>2</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="3">
-        <f>$D$1*C17</f>
-        <v>6</v>
-      </c>
-      <c r="G17" s="6"/>
-    </row>
-    <row r="18" spans="1:7">
+        <f>D15+30</f>
+        <v>84</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="3"/>
       <c r="B18" s="3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C18" s="3">
-        <v>10</v>
+        <f xml:space="preserve"> ROUNDUP($C$17/8, 0)</f>
+        <v>11</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E18" s="3">
-        <f t="shared" ref="E18:E19" si="2">$D$1*C18</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <f>C18*$D$1</f>
+        <v>11</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="3"/>
-      <c r="B19" s="3">
-        <v>1</v>
-      </c>
-      <c r="C19" s="3">
-        <v>18</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="3">
-        <f>$D$1*C19</f>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="3"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="5"/>
       <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" spans="1:10">
       <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+    </row>
+    <row r="22" spans="1:10">
       <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="B23" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="3">
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="B24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="3">
         <f>D15/2</f>
         <v>27</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:10">
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:7">
-      <c r="B26" s="1" t="s">
-        <v>20</v>
-      </c>
+    <row r="26" spans="1:10">
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:10">
       <c r="B27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="1">
-        <v>1</v>
-      </c>
-      <c r="D27" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="B28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="3">
+        <f>$D$1*C28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="B29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E27" s="3">
-        <f t="shared" ref="E27:E40" si="3">$D$1*C27</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="B28" s="1" t="s">
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="1">
-        <v>1</v>
-      </c>
-      <c r="E28" s="3">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="B29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="1">
-        <v>1</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>25</v>
-      </c>
       <c r="E29" s="3">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <f t="shared" ref="E29:E34" si="2">$D$1*C29</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="B30" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="B31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E30" s="3">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="B31" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" s="1">
-        <v>1</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>28</v>
-      </c>
       <c r="E31" s="3">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="B32" s="1" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="E32" s="3">
-        <f t="shared" si="3"/>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C33" s="1">
-        <v>3</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="E33" s="3">
-        <f t="shared" si="3"/>
-        <v>9</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="C34" s="1">
+        <v>3</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="3">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5">
+      <c r="B35" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D17" r:id="rId1"/>
-    <hyperlink ref="D18" r:id="rId2"/>
-    <hyperlink ref="D19" r:id="rId3"/>
-    <hyperlink ref="D27" r:id="rId4"/>
-    <hyperlink ref="D5" r:id="rId5"/>
-    <hyperlink ref="D6" r:id="rId6"/>
-    <hyperlink ref="D29" r:id="rId7"/>
-    <hyperlink ref="D4" r:id="rId8"/>
-    <hyperlink ref="D30" r:id="rId9"/>
-    <hyperlink ref="D31" r:id="rId10"/>
-    <hyperlink ref="D3" r:id="rId11"/>
-    <hyperlink ref="D32" r:id="rId12"/>
-    <hyperlink ref="D33" r:id="rId13"/>
+    <hyperlink ref="D28" r:id="rId1"/>
+    <hyperlink ref="D5" r:id="rId2"/>
+    <hyperlink ref="D6" r:id="rId3"/>
+    <hyperlink ref="D4" r:id="rId4"/>
+    <hyperlink ref="D31" r:id="rId5"/>
+    <hyperlink ref="D32" r:id="rId6"/>
+    <hyperlink ref="D3" r:id="rId7"/>
+    <hyperlink ref="D33" r:id="rId8"/>
+    <hyperlink ref="D34" r:id="rId9"/>
+    <hyperlink ref="D29" r:id="rId10"/>
+    <hyperlink ref="I9" r:id="rId11"/>
+    <hyperlink ref="I10" r:id="rId12"/>
+    <hyperlink ref="I11" r:id="rId13"/>
+    <hyperlink ref="I12" r:id="rId14"/>
+    <hyperlink ref="I14" r:id="rId15"/>
+    <hyperlink ref="I15" r:id="rId16"/>
+    <hyperlink ref="I8" r:id="rId17"/>
+    <hyperlink ref="I13" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId19"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
converted to single ground, part list propably doneish
</commit_message>
<xml_diff>
--- a/parts.xlsx
+++ b/parts.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
   <si>
     <t>NUMBER OF BOARDS</t>
   </si>
@@ -108,9 +108,6 @@
     <t>piezzo 1kR</t>
   </si>
   <si>
-    <t>LED 330 R</t>
-  </si>
-  <si>
     <t>https://www.tme.eu/cz/details/bpt-14x/piezosireny-s-generatorem/bestar/bpt14x/</t>
   </si>
   <si>
@@ -118,6 +115,27 @@
   </si>
   <si>
     <t>HEADER 8</t>
+  </si>
+  <si>
+    <t>https://www.gme.cz/ru-22k-0207-0-25w-5</t>
+  </si>
+  <si>
+    <t>22kR</t>
+  </si>
+  <si>
+    <t>https://www.gme.cz/mikrospinac-tc-0105-t</t>
+  </si>
+  <si>
+    <t>https://www.gme.cz/rm-1k-0207-0-6w-1</t>
+  </si>
+  <si>
+    <t>https://www.gme.cz/rm-150r-0207-0-6w-1</t>
+  </si>
+  <si>
+    <t>150R</t>
+  </si>
+  <si>
+    <t>LED 150 R</t>
   </si>
 </sst>
 </file>
@@ -141,7 +159,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,6 +184,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -183,7 +207,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -207,6 +231,21 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -506,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -550,7 +589,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="E3" s="3">
         <f>$D$1*C3</f>
@@ -612,7 +651,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="3"/>
       <c r="G7" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -629,7 +668,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="3"/>
       <c r="G8" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H8" s="7">
         <f xml:space="preserve"> ROUNDUP($C$17/8, 0)*$D$1</f>
@@ -656,14 +695,14 @@
       </c>
       <c r="E9" s="3"/>
       <c r="G9" s="7" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="H9" s="7">
-        <f>E3+E4+E34+E31</f>
-        <v>11</v>
+        <f>E3+E4</f>
+        <v>7</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="J9" s="7"/>
     </row>
@@ -771,7 +810,7 @@
         <v>1</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J13" s="7"/>
     </row>
@@ -793,8 +832,8 @@
         <f>E32</f>
         <v>1</v>
       </c>
-      <c r="I14" s="6" t="s">
-        <v>18</v>
+      <c r="I14" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="J14" s="7"/>
     </row>
@@ -815,7 +854,7 @@
         <f>E33</f>
         <v>1</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="10" t="s">
         <v>20</v>
       </c>
       <c r="J15" s="7"/>
@@ -828,9 +867,16 @@
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
+      <c r="G16" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="12">
+        <f>E31</f>
+        <v>1</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>36</v>
+      </c>
       <c r="J16" s="7"/>
     </row>
     <row r="17" spans="1:10">
@@ -844,9 +890,16 @@
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
+      <c r="G17" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="12">
+        <f>E34</f>
+        <v>1</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>37</v>
+      </c>
       <c r="J17" s="7"/>
     </row>
     <row r="18" spans="1:10">
@@ -970,7 +1023,7 @@
         <v>1</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E30" s="3">
         <f t="shared" si="2"/>
@@ -1023,18 +1076,18 @@
       </c>
     </row>
     <row r="34" spans="2:5">
-      <c r="B34" s="1" t="s">
-        <v>30</v>
+      <c r="B34" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="C34" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E34" s="3">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="2:5">
@@ -1050,21 +1103,19 @@
     <hyperlink ref="D4" r:id="rId4"/>
     <hyperlink ref="D31" r:id="rId5"/>
     <hyperlink ref="D32" r:id="rId6"/>
-    <hyperlink ref="D3" r:id="rId7"/>
-    <hyperlink ref="D33" r:id="rId8"/>
-    <hyperlink ref="D34" r:id="rId9"/>
-    <hyperlink ref="D29" r:id="rId10"/>
-    <hyperlink ref="I9" r:id="rId11"/>
-    <hyperlink ref="I10" r:id="rId12"/>
-    <hyperlink ref="I11" r:id="rId13"/>
-    <hyperlink ref="I12" r:id="rId14"/>
-    <hyperlink ref="I14" r:id="rId15"/>
-    <hyperlink ref="I15" r:id="rId16"/>
-    <hyperlink ref="I8" r:id="rId17"/>
-    <hyperlink ref="I13" r:id="rId18"/>
+    <hyperlink ref="D33" r:id="rId7"/>
+    <hyperlink ref="D34" r:id="rId8"/>
+    <hyperlink ref="D29" r:id="rId9"/>
+    <hyperlink ref="I10" r:id="rId10"/>
+    <hyperlink ref="I11" r:id="rId11"/>
+    <hyperlink ref="I12" r:id="rId12"/>
+    <hyperlink ref="I8" r:id="rId13"/>
+    <hyperlink ref="I13" r:id="rId14"/>
+    <hyperlink ref="I15" r:id="rId15"/>
+    <hyperlink ref="I17" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId17"/>
 </worksheet>
 </file>
 

</xml_diff>